<commit_message>
Parameters to be analyzed from 2009 to 2019 more completed
</commit_message>
<xml_diff>
--- a/ParametersToBeAnalyzed_Nat.xlsx
+++ b/ParametersToBeAnalyzed_Nat.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nattz\Desktop\Data Challenge\datachallenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEAEF7FD-6D11-492B-B693-4167D00FB1D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D27D817-DC5A-44DD-9E83-AA80C0100886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E882E0C4-126D-462D-964E-A4B9B80440BD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Available parameters" sheetId="1" r:id="rId1"/>
+    <sheet name="Parameters to be studied" sheetId="2" r:id="rId2"/>
+    <sheet name="Matrices" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
-  <si>
-    <t>['Shares (Basic)',</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="83">
   <si>
     <t xml:space="preserve"> 'Shares (Diluted)',</t>
   </si>
@@ -85,9 +84,6 @@
   </si>
   <si>
     <t xml:space="preserve"> 'Retained Earnings',</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'Total Equity']</t>
   </si>
   <si>
     <t>Diluted shares are those shares or share stock that will be available to the company after undergoing all the sources of conversions are exercised like Employee Stock Option Plans, Convertible bond conversions</t>
@@ -204,17 +200,414 @@
     <t xml:space="preserve"> 'Income Tax (Expense) Benefit, Net',</t>
   </si>
   <si>
-    <t xml:space="preserve"> 'Net Extraordinary Gains (Losses)']</t>
-  </si>
-  <si>
     <t>US Income</t>
+  </si>
+  <si>
+    <t>Determined By</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terminology </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company Sectors </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Total Equity'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Net Extraordinary Gains (Losses)'</t>
+  </si>
+  <si>
+    <r>
+      <t>Noncurrent assets are </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FF202124"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>a company's long-term investments for which the full value will not be realized within the accounting year</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF202124"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>. </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">How well the organization is capable to meet its short-term financial obligation? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How well the organization is capable to meet its long-term financial obligation? </t>
+  </si>
+  <si>
+    <t>2. Liquidity ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Profitability </t>
+  </si>
+  <si>
+    <t>How can I use the available data?</t>
+  </si>
+  <si>
+    <t>Which story will I tell?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Solvency ratio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.1 Gearing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">assessment whether the organization will be able to receive external funding to grow </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definition/Goal/Objective </t>
+  </si>
+  <si>
+    <t>to compare organizational´s external funding with that invested in it by its shareholders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good to use when </t>
+  </si>
+  <si>
+    <t xml:space="preserve">low ratio is desirable as this will provide scope for further borrowing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.2 debt to asset ratio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">assessing whether the level of debt is reasonable in relation to the value of organization asset </t>
+  </si>
+  <si>
+    <t>low ratio is more favourable by the lenders</t>
+  </si>
+  <si>
+    <r>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>long-term debt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>equity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- see balance sheet</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">2.1Working Capital Ratio (or current ratio) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">a low figure shows the organization may be unable to pay its bill in the future </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assessment </t>
+  </si>
+  <si>
+    <t>It shows how the organization can pay back short-term liabilities with its short-term assets</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">How well the organizations is managing its capital? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+represents a company's ability to pay its current liabilities with its current assets. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Working capital is an important measure of financial health</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> since creditors can </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>measure a company's ability to pay off its debts within a year</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+Working capital represents the difference between a firm’s current assets and current liabilities. </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">What are my hypotheses? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Below table shows ratios that are used to determine how healthy the organizations are </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">from available data (Income, Balance and Cashflow sheets), the following (green colored) parameters are assessable 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">debt </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF404040"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">of ratio, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>R&amp;D expenses</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF404040"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, expenses in public sectors, numbers of employees, 
+level of globalization, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>dividend give back to investors</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF404040"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">/announce/actually paid to investors, 
+level supported by government, tax benefits ratio marketing expenses, numbers of stores, 
+management bonus, amount of taxes payment, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">earning </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">What characteristics assist in company (in various sectors and in short-term and long-term bases) survivalabilities during ….. 
+we started with the following hypotheses: 
+debt of ratio, R&amp;D expenses, expenses in public sectors, numbers of employees, 
+level of globalization, dividend give back to investors/announce/actually paid to investors, 
+level supported by government, tax benefits ratio marketing expenses, numbers of stores, 
+management bonus, amount of taxes payment, earning </t>
+  </si>
+  <si>
+    <r>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>current asset</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>current liabilities</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) 
+- current asset can be found in the balance sheet </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>long-term debt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>total asset</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- see balance sheet</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,15 +643,60 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Var(--jp-code-font-family)"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Var(--jp-code-font-family)"/>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF111111"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF404040"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF404040"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -267,30 +705,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -298,51 +724,234 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -661,222 +1270,435 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="54.453125" customWidth="1"/>
-    <col min="2" max="2" width="46" style="6" customWidth="1"/>
-    <col min="3" max="3" width="49.7265625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="73" customWidth="1"/>
+    <col min="1" max="1" width="54.453125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="46" style="17" customWidth="1"/>
+    <col min="3" max="3" width="49.7265625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="90" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="36" customHeight="1">
+      <c r="A3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="B5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="36" customHeight="1">
-      <c r="A3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="13" t="s">
+      <c r="C5" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="13" t="s">
+      <c r="C6" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B7" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="13" t="s">
+      <c r="C7" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B8" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="13" t="s">
+      <c r="C8" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B9" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="8" t="s">
+      <c r="C9" s="11" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="13" t="s">
+      <c r="C12" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B13" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="13" t="s">
+      <c r="C13" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B14" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="9" t="s">
+      <c r="C14" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="9" t="s">
+      <c r="C15" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="B16" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="9" t="s">
+      <c r="C16" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="B16" s="10" t="s">
+      <c r="C17" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="B17" s="7" t="s">
+      <c r="C18" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3">
-      <c r="B18" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3">
-      <c r="B19" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>17</v>
+      <c r="C19" s="11" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB05FD6-BA6F-4995-9BDC-B97B5D1FB33C}">
+  <dimension ref="B2:F15"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="60" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="3"/>
+    <col min="2" max="2" width="42.7265625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="86.453125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="38.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="41.36328125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="33.54296875" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" ht="168.5" customHeight="1">
+      <c r="B2" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="2:6" ht="117" customHeight="1">
+      <c r="B3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="2:6" ht="48" customHeight="1" thickBot="1">
+      <c r="B4" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="20"/>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="21"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="24"/>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="25"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="24"/>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="24"/>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="21"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="24"/>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="30"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="31"/>
+    </row>
+    <row r="12" spans="2:6" ht="108.5">
+      <c r="B12" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="38"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="39"/>
+    </row>
+    <row r="14" spans="2:6" ht="55" customHeight="1">
+      <c r="B14" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="44" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="64" customHeight="1" thickBot="1">
+      <c r="B15" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="46"/>
+      <c r="D15" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="49" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B5:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC6BB14D-3A9F-4F6E-8684-C2E6AF4AD7EE}">
+  <dimension ref="B2:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="50.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2">
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="74" customHeight="1">
+      <c r="B4" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>